<commit_message>
built ranked_table ~ needs progress bar
</commit_message>
<xml_diff>
--- a/Global_YouTube_Statistics.xlsx
+++ b/Global_YouTube_Statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data Analytics\youtube_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98F8684B-7932-4E47-A865-52E95B8EEAAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17D9464-45AB-437D-A71E-B5D418A99EE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global_YouTube_Statistics" sheetId="1" r:id="rId1"/>
@@ -3898,7 +3898,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4734,11 +4734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AB1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
wrote preprocessing script in notebook in Scripts~dropped and reshaped df
</commit_message>
<xml_diff>
--- a/Global_YouTube_Statistics.xlsx
+++ b/Global_YouTube_Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data Analytics\youtube_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17D9464-45AB-437D-A71E-B5D418A99EE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C15A26E-0141-459A-AE0B-A42534962325}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4737,38 +4737,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34.5546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>